<commit_message>
Added statistical model checking to classification
</commit_message>
<xml_diff>
--- a/classification/classification-nomenclature.xlsx
+++ b/classification/classification-nomenclature.xlsx
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="98">
   <si>
     <t>Analysis Method</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t>composition-based implementation</t>
+  </si>
+  <si>
+    <t>statistical model checking</t>
   </si>
 </sst>
 </file>
@@ -839,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,27 +1187,30 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>97</v>
+      </c>
       <c r="G20" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>72</v>
-      </c>
       <c r="G21" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="G22" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
       <c r="G23" t="s">
         <v>93</v>
       </c>

</xml_diff>